<commit_message>
Actualizacion de historias de usuario MVP
</commit_message>
<xml_diff>
--- a/Documentacion/HistoriasdeUsuario.xlsx
+++ b/Documentacion/HistoriasdeUsuario.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Propietario\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\juanc\Desktop\INFO264_Proyecto\Documentacion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{F809EA45-EF73-4A34-AC13-30963EDF9F13}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B56E5DD-C7FC-430B-9EE2-5FAAFC9A1735}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" xr2:uid="{38888050-83B5-4BB9-AE0B-EBF73E1C02A2}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20496" windowHeight="7548" xr2:uid="{38888050-83B5-4BB9-AE0B-EBF73E1C02A2}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="42">
   <si>
     <t>Enunciado de la Historia</t>
   </si>
@@ -69,15 +69,6 @@
     <t>Acceso a redes sociales</t>
   </si>
   <si>
-    <t>En caso de que el usuario inicie la plataforma le solicite correo y contraseña a utilizar</t>
-  </si>
-  <si>
-    <t>En caso de que el usuario se llegue a equivocar al ingresar la informacion se le solicita nuesvamente</t>
-  </si>
-  <si>
-    <t>En caso de que la validacion sea correcta el usuario accedera a sus cuentas de redes sociales</t>
-  </si>
-  <si>
     <t>Necesito Enviar post a 3 redes sociales</t>
   </si>
   <si>
@@ -93,14 +84,80 @@
     <t>Post Instagram</t>
   </si>
   <si>
-    <t>En caso de que el usuario seleccione esta red podra realizar un post en ella</t>
+    <t>Rol</t>
+  </si>
+  <si>
+    <t>Gerenta</t>
+  </si>
+  <si>
+    <t>Al dar inicio a a aplicación</t>
+  </si>
+  <si>
+    <t>Necesito adjuntar foto</t>
+  </si>
+  <si>
+    <t>Informacion mas detallada de la noticia</t>
+  </si>
+  <si>
+    <t>Adjuntar</t>
+  </si>
+  <si>
+    <t>hacer click en postear por Facebook</t>
+  </si>
+  <si>
+    <t>hacer click en postear por Twitter</t>
+  </si>
+  <si>
+    <t>hacer click en postear por Instagram</t>
+  </si>
+  <si>
+    <t>Yo Claudia necesito realizar un post en Twitter</t>
+  </si>
+  <si>
+    <t>Yo Claudia necesito realizar un post en Facebook</t>
+  </si>
+  <si>
+    <t>Yo Claudia necesito realizar un post en Instagram</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Yo claudia necesito utilizar las cuentas de correo  de la empresa y quiero solicite correo y contraseña </t>
+  </si>
+  <si>
+    <t>Yo claudia en caso de que me equivoque  necesito saber donde me equivoque</t>
+  </si>
+  <si>
+    <t>Yo claudia necesito poder tener acceso a las redes sociales para poder postear</t>
+  </si>
+  <si>
+    <t>Crear Noticia</t>
+  </si>
+  <si>
+    <t>crear contexto de la noticia</t>
+  </si>
+  <si>
+    <t>Crear</t>
+  </si>
+  <si>
+    <t>Yo claudia necesito poder adjuntar audio o imágenes</t>
+  </si>
+  <si>
+    <t>hacer click en la herramienta de adjuntar</t>
+  </si>
+  <si>
+    <t>Yo claudia quiero poder crear una noticia y poder postearla</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Se crea la noticia con titular su texto informativo </t>
+  </si>
+  <si>
+    <t>y se envia a las redes sociales del usuario</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -110,6 +167,14 @@
     </font>
     <font>
       <sz val="9"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -142,7 +207,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -253,11 +318,48 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
@@ -286,6 +388,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -295,6 +400,34 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -609,39 +742,40 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{62CE16C3-D0A0-4F73-A8E2-56FABC90615E}">
-  <dimension ref="A2:I15"/>
+  <dimension ref="A2:J34"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+      <selection activeCell="G34" sqref="G34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.7109375" customWidth="1"/>
-    <col min="2" max="2" width="26.85546875" customWidth="1"/>
-    <col min="3" max="3" width="19.140625" customWidth="1"/>
-    <col min="4" max="4" width="13.42578125" customWidth="1"/>
-    <col min="5" max="5" width="30.42578125" customWidth="1"/>
-    <col min="6" max="6" width="101.42578125" customWidth="1"/>
-    <col min="7" max="7" width="22.5703125" customWidth="1"/>
+    <col min="1" max="1" width="15.6640625" customWidth="1"/>
+    <col min="2" max="2" width="26.88671875" customWidth="1"/>
+    <col min="3" max="4" width="19.109375" customWidth="1"/>
+    <col min="5" max="5" width="13.44140625" customWidth="1"/>
+    <col min="6" max="6" width="30.44140625" customWidth="1"/>
+    <col min="7" max="7" width="90" customWidth="1"/>
+    <col min="8" max="8" width="43.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="8" t="s">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A2" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="8"/>
-      <c r="C2" s="8"/>
-      <c r="D2" s="8"/>
-      <c r="E2" s="8" t="s">
+      <c r="B2" s="16"/>
+      <c r="C2" s="16"/>
+      <c r="D2" s="16"/>
+      <c r="E2" s="16"/>
+      <c r="F2" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="F2" s="8"/>
-      <c r="G2" s="8"/>
-      <c r="H2" s="1"/>
+      <c r="G2" s="16"/>
+      <c r="H2" s="16"/>
       <c r="I2" s="1"/>
-    </row>
-    <row r="3" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J2" s="1"/>
+    </row>
+    <row r="3" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="6" t="s">
         <v>2</v>
       </c>
@@ -651,84 +785,95 @@
       <c r="C3" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="7" t="s">
+      <c r="D3" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="E3" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="F3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="F3" s="2" t="s">
+      <c r="G3" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="G3" s="2" t="s">
+      <c r="H3" s="2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="9">
         <v>1</v>
       </c>
-      <c r="B4" s="16" t="s">
+      <c r="B4" s="17" t="s">
         <v>9</v>
       </c>
       <c r="C4" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="D4" s="3">
+      <c r="D4" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="E4" s="3">
         <v>1</v>
       </c>
-      <c r="E4" s="5" t="s">
+      <c r="F4" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="F4" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="G4" s="4"/>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G4" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="H4" s="21" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" s="11"/>
-      <c r="B5" s="17"/>
+      <c r="B5" s="18"/>
       <c r="C5" s="14"/>
-      <c r="D5" s="4">
+      <c r="D5" s="18"/>
+      <c r="E5" s="4">
         <v>2</v>
       </c>
-      <c r="E5" s="4" t="s">
+      <c r="F5" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="F5" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="G5" s="4"/>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G5" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="H5" s="22"/>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" s="12"/>
-      <c r="B6" s="18"/>
+      <c r="B6" s="19"/>
       <c r="C6" s="15"/>
-      <c r="D6" s="4">
+      <c r="D6" s="19"/>
+      <c r="E6" s="4">
         <v>3</v>
       </c>
-      <c r="E6" s="4" t="s">
+      <c r="F6" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="F6" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="G6" s="4"/>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="8" t="s">
+      <c r="G6" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="H6" s="23"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A10" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="B10" s="8"/>
-      <c r="C10" s="8"/>
-      <c r="D10" s="8"/>
-      <c r="E10" s="8" t="s">
+      <c r="B10" s="16"/>
+      <c r="C10" s="16"/>
+      <c r="D10" s="16"/>
+      <c r="E10" s="16"/>
+      <c r="F10" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="F10" s="8"/>
-      <c r="G10" s="8"/>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G10" s="16"/>
+      <c r="H10" s="16"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>2</v>
       </c>
@@ -738,91 +883,314 @@
       <c r="C11" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D11" s="7" t="s">
+      <c r="D11" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="E11" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="E11" s="2" t="s">
+      <c r="F11" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="F11" s="2" t="s">
+      <c r="G11" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="G11" s="2" t="s">
+      <c r="H11" s="2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="9">
         <v>2</v>
       </c>
-      <c r="B12" s="16" t="s">
+      <c r="B12" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="C12" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="D12" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="E12" s="3">
+        <v>1</v>
+      </c>
+      <c r="F12" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="G12" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="H12" s="4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A13" s="11"/>
+      <c r="B13" s="18"/>
+      <c r="C13" s="14"/>
+      <c r="D13" s="18"/>
+      <c r="E13" s="4">
+        <v>2</v>
+      </c>
+      <c r="F13" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="C12" s="13" t="s">
+      <c r="G13" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="H13" s="4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A14" s="11"/>
+      <c r="B14" s="18"/>
+      <c r="C14" s="14"/>
+      <c r="D14" s="18"/>
+      <c r="E14" s="4">
+        <v>3</v>
+      </c>
+      <c r="F14" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="D12" s="3">
+      <c r="G14" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="H14" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A15" s="10"/>
+      <c r="B15" s="19"/>
+      <c r="C15" s="15"/>
+      <c r="D15" s="19"/>
+      <c r="E15" s="4"/>
+      <c r="F15" s="4"/>
+      <c r="G15" s="4"/>
+      <c r="H15" s="4"/>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A18" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="B18" s="16"/>
+      <c r="C18" s="16"/>
+      <c r="D18" s="16"/>
+      <c r="E18" s="16"/>
+      <c r="F18" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="E12" s="5" t="s">
+      <c r="G18" s="16"/>
+      <c r="H18" s="16"/>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A19" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D19" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="F12" s="4" t="s">
+      <c r="E19" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="F19" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G19" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="H19" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A20" s="9">
+        <v>3</v>
+      </c>
+      <c r="B20" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="G12" s="4"/>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" s="11"/>
-      <c r="B13" s="17"/>
-      <c r="C13" s="14"/>
-      <c r="D13" s="4">
+      <c r="C20" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="D20" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="E20" s="3">
+        <v>1</v>
+      </c>
+      <c r="F20" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="G20" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="H20" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A21" s="11"/>
+      <c r="B21" s="18"/>
+      <c r="C21" s="14"/>
+      <c r="D21" s="18"/>
+      <c r="E21" s="4"/>
+      <c r="F21" s="4"/>
+      <c r="G21" s="4"/>
+      <c r="H21" s="4"/>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A22" s="11"/>
+      <c r="B22" s="18"/>
+      <c r="C22" s="14"/>
+      <c r="D22" s="18"/>
+      <c r="E22" s="4"/>
+      <c r="F22" s="4"/>
+      <c r="G22" s="4"/>
+      <c r="H22" s="4"/>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A23" s="10"/>
+      <c r="B23" s="19"/>
+      <c r="C23" s="15"/>
+      <c r="D23" s="19"/>
+      <c r="E23" s="4"/>
+      <c r="F23" s="4"/>
+      <c r="G23" s="4"/>
+      <c r="H23" s="4"/>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A26" s="24" t="s">
+        <v>0</v>
+      </c>
+      <c r="B26" s="26"/>
+      <c r="C26" s="26"/>
+      <c r="D26" s="26"/>
+      <c r="E26" s="25"/>
+      <c r="F26" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="G26" s="8"/>
+      <c r="H26" s="8"/>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A27" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E13" s="4" t="s">
+      <c r="B27" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D27" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="E27" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="F27" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G27" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="H27" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A28" s="9">
+        <v>4</v>
+      </c>
+      <c r="B28" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="C28" s="17" t="s">
+        <v>35</v>
+      </c>
+      <c r="D28" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="F13" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="G13" s="4"/>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" s="11"/>
-      <c r="B14" s="17"/>
-      <c r="C14" s="14"/>
-      <c r="D14" s="4">
-        <v>3</v>
-      </c>
-      <c r="E14" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="F14" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="G14" s="4"/>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15" s="10"/>
-      <c r="B15" s="18"/>
-      <c r="C15" s="15"/>
-      <c r="D15" s="4"/>
-      <c r="E15" s="4"/>
-      <c r="F15" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="G15" s="4"/>
+      <c r="E28" s="3">
+        <v>1</v>
+      </c>
+      <c r="F28" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="G28" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="H28" s="27" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A29" s="11"/>
+      <c r="B29" s="18"/>
+      <c r="C29" s="18"/>
+      <c r="D29" s="18"/>
+      <c r="E29" s="4"/>
+      <c r="F29" s="4"/>
+      <c r="G29" s="4"/>
+      <c r="H29" s="28" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A30" s="11"/>
+      <c r="B30" s="18"/>
+      <c r="C30" s="18"/>
+      <c r="D30" s="18"/>
+      <c r="E30" s="4"/>
+      <c r="F30" s="4"/>
+      <c r="G30" s="4"/>
+      <c r="H30" s="22"/>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A31" s="10"/>
+      <c r="B31" s="19"/>
+      <c r="C31" s="19"/>
+      <c r="D31" s="19"/>
+      <c r="E31" s="4"/>
+      <c r="F31" s="4"/>
+      <c r="G31" s="4"/>
+      <c r="H31" s="23"/>
+    </row>
+    <row r="34" spans="7:7" x14ac:dyDescent="0.3">
+      <c r="G34" s="29"/>
     </row>
   </sheetData>
-  <mergeCells count="8">
+  <mergeCells count="21">
+    <mergeCell ref="C28:C31"/>
+    <mergeCell ref="D28:D31"/>
+    <mergeCell ref="A26:E26"/>
+    <mergeCell ref="B28:B31"/>
+    <mergeCell ref="H30:H31"/>
+    <mergeCell ref="B20:B23"/>
+    <mergeCell ref="C20:C23"/>
+    <mergeCell ref="D4:D6"/>
+    <mergeCell ref="D12:D15"/>
+    <mergeCell ref="D20:D23"/>
+    <mergeCell ref="A2:E2"/>
+    <mergeCell ref="F2:H2"/>
+    <mergeCell ref="B4:B6"/>
+    <mergeCell ref="A18:E18"/>
+    <mergeCell ref="F18:H18"/>
+    <mergeCell ref="H4:H6"/>
     <mergeCell ref="C4:C6"/>
-    <mergeCell ref="A10:D10"/>
-    <mergeCell ref="E10:G10"/>
+    <mergeCell ref="A10:E10"/>
+    <mergeCell ref="F10:H10"/>
     <mergeCell ref="B12:B15"/>
     <mergeCell ref="C12:C15"/>
-    <mergeCell ref="A2:D2"/>
-    <mergeCell ref="E2:G2"/>
-    <mergeCell ref="B4:B6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>